<commit_message>
Fully working version (not correctly working data)
</commit_message>
<xml_diff>
--- a/Основы Машинного обучения/Лаб1FeatureSpace/data.xlsx
+++ b/Основы Машинного обучения/Лаб1FeatureSpace/data.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Учёба\4 курс\LabsAntonAndrew\Основы Машинного обучения\Лаб1FeatureSpace\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29500A21-9441-4950-9FEE-56BD18EB8AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="11">
   <si>
     <t>Node</t>
   </si>
@@ -42,12 +48,18 @@
   <si>
     <t>u (Q)</t>
   </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,47 +111,76 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>u(S)</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet1'!$H$2</c:f>
+              <c:f>Sheet1!$H$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.2</c:v>
+                  <c:v>9.0909090909090898E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F656-4F29-A8E1-73718074B023}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -147,18 +188,24 @@
           <c:tx>
             <c:v>u(Э)</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet1'!$I$2</c:f>
+              <c:f>Sheet1!$I$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.2</c:v>
+                  <c:v>9.0909090909090898E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F656-4F29-A8E1-73718074B023}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -166,19 +213,34 @@
           <c:tx>
             <c:v>u(L)</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet1'!$J$2</c:f>
+              <c:f>Sheet1!$J$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.2</c:v>
+                  <c:v>9.0909090909090898E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F656-4F29-A8E1-73718074B023}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="50010001"/>
         <c:axId val="50010002"/>
       </c:barChart>
@@ -187,22 +249,29 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50010002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010001"/>
         <c:crosses val="autoZero"/>
@@ -211,9 +280,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -240,7 +311,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -259,9 +336,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -299,9 +376,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -333,9 +410,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -367,9 +462,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -542,14 +655,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -588,29 +703,29 @@
       <c r="C2">
         <v>4</v>
       </c>
-      <c r="D2">
-        <v>0</v>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>3.16227766016838</v>
       </c>
       <c r="F2">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="H2">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="I2">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="J2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>9.0909090909090898E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -620,14 +735,14 @@
       <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3">
-        <v>0</v>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>3.16227766016838</v>
       </c>
       <c r="F3">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
@@ -642,7 +757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -652,14 +767,14 @@
       <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4">
-        <v>0</v>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>3.16227766016838</v>
       </c>
       <c r="F4">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
@@ -674,7 +789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -684,14 +799,14 @@
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>0</v>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>3.16227766016838</v>
       </c>
       <c r="F5">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
@@ -706,7 +821,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -716,14 +831,14 @@
       <c r="C6">
         <v>3</v>
       </c>
-      <c r="D6">
-        <v>0</v>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>3.16227766016838</v>
       </c>
       <c r="F6">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
@@ -738,7 +853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -748,14 +863,14 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7">
-        <v>1</v>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>3.6055512754639891</v>
       </c>
       <c r="F7">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
@@ -770,7 +885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -780,14 +895,14 @@
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8">
-        <v>1</v>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>3.6055512754639891</v>
       </c>
       <c r="F8">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
@@ -802,7 +917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -812,14 +927,14 @@
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9">
-        <v>1</v>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>3.6055512754639891</v>
       </c>
       <c r="F9">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
@@ -834,7 +949,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -844,14 +959,14 @@
       <c r="C10">
         <v>3</v>
       </c>
-      <c r="D10">
-        <v>1</v>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>3.6055512754639891</v>
       </c>
       <c r="F10">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
@@ -866,7 +981,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -876,14 +991,14 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11">
-        <v>1</v>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>3.6055512754639891</v>
       </c>
       <c r="F11">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="G11" t="s">
         <v>5</v>
@@ -898,7 +1013,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -908,14 +1023,14 @@
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12">
-        <v>2</v>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>2.2360679774997898</v>
       </c>
       <c r="F12">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="G12" t="s">
         <v>5</v>
@@ -930,7 +1045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -940,14 +1055,14 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13">
-        <v>2</v>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>2.2360679774997898</v>
       </c>
       <c r="F13">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="G13" t="s">
         <v>5</v>
@@ -962,7 +1077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -972,14 +1087,14 @@
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14">
-        <v>2</v>
+      <c r="D14" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>2.2360679774997898</v>
       </c>
       <c r="F14">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
@@ -994,7 +1109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1004,14 +1119,14 @@
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15">
-        <v>2</v>
+      <c r="D15" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>2.2360679774997898</v>
       </c>
       <c r="F15">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="G15" t="s">
         <v>5</v>
@@ -1026,7 +1141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1036,14 +1151,14 @@
       <c r="C16">
         <v>2</v>
       </c>
-      <c r="D16">
-        <v>2</v>
+      <c r="D16" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>2.2360679774997898</v>
       </c>
       <c r="F16">
-        <v>0.2</v>
+        <v>9.0909090909090898E-2</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>

</xml_diff>